<commit_message>
Old testing fixed and ethics results
</commit_message>
<xml_diff>
--- a/Documentation/Ethical Testing/SUS Results.xlsx
+++ b/Documentation/Ethical Testing/SUS Results.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\oliversimpson\Documents\Industrial Project\Ethical Testing\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\asus\Documents\GitHub\CranewareProject\Documentation\Ethical Testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6F8F054-55D3-4FD4-9F55-405669FE592F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Participant No</t>
   </si>
@@ -60,12 +61,15 @@
   </si>
   <si>
     <t>Total Score</t>
+  </si>
+  <si>
+    <t>Average</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -376,11 +380,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:L9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M4" sqref="M4"/>
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -427,6 +431,280 @@
         <v>11</v>
       </c>
     </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>9</v>
+      </c>
+      <c r="C2">
+        <v>10</v>
+      </c>
+      <c r="D2">
+        <v>10</v>
+      </c>
+      <c r="E2">
+        <v>10</v>
+      </c>
+      <c r="F2">
+        <v>8</v>
+      </c>
+      <c r="G2">
+        <v>5</v>
+      </c>
+      <c r="H2">
+        <v>10</v>
+      </c>
+      <c r="I2">
+        <v>6</v>
+      </c>
+      <c r="J2">
+        <v>9</v>
+      </c>
+      <c r="K2">
+        <v>10</v>
+      </c>
+      <c r="L2">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>4</v>
+      </c>
+      <c r="B3">
+        <v>9</v>
+      </c>
+      <c r="C3">
+        <v>8</v>
+      </c>
+      <c r="D3">
+        <v>7</v>
+      </c>
+      <c r="E3">
+        <v>10</v>
+      </c>
+      <c r="F3">
+        <v>8</v>
+      </c>
+      <c r="G3">
+        <v>6</v>
+      </c>
+      <c r="H3">
+        <v>9</v>
+      </c>
+      <c r="I3">
+        <v>10</v>
+      </c>
+      <c r="J3">
+        <v>8</v>
+      </c>
+      <c r="K3">
+        <v>8</v>
+      </c>
+      <c r="L3">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>8</v>
+      </c>
+      <c r="B4">
+        <v>10</v>
+      </c>
+      <c r="C4">
+        <v>10</v>
+      </c>
+      <c r="D4">
+        <v>10</v>
+      </c>
+      <c r="E4">
+        <v>10</v>
+      </c>
+      <c r="F4">
+        <v>9</v>
+      </c>
+      <c r="G4">
+        <v>10</v>
+      </c>
+      <c r="H4">
+        <v>10</v>
+      </c>
+      <c r="I4">
+        <v>10</v>
+      </c>
+      <c r="J4">
+        <v>10</v>
+      </c>
+      <c r="K4">
+        <v>10</v>
+      </c>
+      <c r="L4">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>12</v>
+      </c>
+      <c r="B5">
+        <v>6</v>
+      </c>
+      <c r="C5">
+        <v>7</v>
+      </c>
+      <c r="D5">
+        <v>7</v>
+      </c>
+      <c r="E5">
+        <v>6</v>
+      </c>
+      <c r="F5">
+        <v>7</v>
+      </c>
+      <c r="G5">
+        <v>9</v>
+      </c>
+      <c r="H5">
+        <v>8</v>
+      </c>
+      <c r="I5">
+        <v>6</v>
+      </c>
+      <c r="J5">
+        <v>9</v>
+      </c>
+      <c r="K5">
+        <v>6</v>
+      </c>
+      <c r="L5">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>13</v>
+      </c>
+      <c r="B6">
+        <v>6</v>
+      </c>
+      <c r="C6">
+        <v>7</v>
+      </c>
+      <c r="D6">
+        <v>7</v>
+      </c>
+      <c r="E6">
+        <v>6</v>
+      </c>
+      <c r="F6">
+        <v>7</v>
+      </c>
+      <c r="G6">
+        <v>9</v>
+      </c>
+      <c r="H6">
+        <v>8</v>
+      </c>
+      <c r="I6">
+        <v>6</v>
+      </c>
+      <c r="J6">
+        <v>9</v>
+      </c>
+      <c r="K6">
+        <v>6</v>
+      </c>
+      <c r="L6">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>14</v>
+      </c>
+      <c r="B7">
+        <v>9</v>
+      </c>
+      <c r="C7">
+        <v>10</v>
+      </c>
+      <c r="D7">
+        <v>8</v>
+      </c>
+      <c r="E7">
+        <v>8</v>
+      </c>
+      <c r="F7">
+        <v>7</v>
+      </c>
+      <c r="G7">
+        <v>10</v>
+      </c>
+      <c r="H7">
+        <v>10</v>
+      </c>
+      <c r="I7">
+        <v>10</v>
+      </c>
+      <c r="J7">
+        <v>10</v>
+      </c>
+      <c r="K7">
+        <v>10</v>
+      </c>
+      <c r="L7">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>16</v>
+      </c>
+      <c r="B8">
+        <v>8</v>
+      </c>
+      <c r="C8">
+        <v>10</v>
+      </c>
+      <c r="D8">
+        <v>10</v>
+      </c>
+      <c r="E8">
+        <v>8</v>
+      </c>
+      <c r="F8">
+        <v>7</v>
+      </c>
+      <c r="G8">
+        <v>10</v>
+      </c>
+      <c r="H8">
+        <v>8</v>
+      </c>
+      <c r="I8">
+        <v>8</v>
+      </c>
+      <c r="J8">
+        <v>10</v>
+      </c>
+      <c r="K8">
+        <v>8</v>
+      </c>
+      <c r="L8">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K9" t="s">
+        <v>12</v>
+      </c>
+      <c r="L9">
+        <v>87.14</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>